<commit_message>
Updated all state election data
</commit_message>
<xml_diff>
--- a/python/Model Election Comparisons.xlsx
+++ b/python/Model Election Comparisons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C1073A-64E9-4CFC-8186-71E03D02539F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6AB9AD-337D-4760-B604-F5F5B6B88D95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25230" yWindow="4950" windowWidth="12570" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25230" yWindow="4950" windowWidth="12570" windowHeight="15900" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019 Fed" sheetId="2" r:id="rId1"/>
@@ -408,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D15B8B6-8389-4FDC-B04C-A068F3734595}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,7 +1583,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,6 +1632,21 @@
       <c r="B3">
         <v>45.55</v>
       </c>
+      <c r="C3">
+        <v>44.06</v>
+      </c>
+      <c r="D3">
+        <v>44.6</v>
+      </c>
+      <c r="E3">
+        <v>45.22</v>
+      </c>
+      <c r="F3">
+        <v>45.85</v>
+      </c>
+      <c r="G3">
+        <v>46.35</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1640,6 +1655,21 @@
       <c r="B4">
         <v>33.380000000000003</v>
       </c>
+      <c r="C4">
+        <v>32.57</v>
+      </c>
+      <c r="D4">
+        <v>33.119999999999997</v>
+      </c>
+      <c r="E4">
+        <v>33.729999999999997</v>
+      </c>
+      <c r="F4">
+        <v>34.36</v>
+      </c>
+      <c r="G4">
+        <v>34.83</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1648,6 +1678,21 @@
       <c r="B5">
         <v>8.65</v>
       </c>
+      <c r="C5">
+        <v>8.86</v>
+      </c>
+      <c r="D5">
+        <v>9.3800000000000008</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>10.63</v>
+      </c>
+      <c r="G5">
+        <v>11.15</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1657,6 +1702,21 @@
         <f>100-SUM(B3:B5)</f>
         <v>12.419999999999987</v>
       </c>
+      <c r="C6">
+        <v>11.27</v>
+      </c>
+      <c r="D6">
+        <v>11.8</v>
+      </c>
+      <c r="E6">
+        <v>12.44</v>
+      </c>
+      <c r="F6">
+        <v>13.03</v>
+      </c>
+      <c r="G6">
+        <v>13.54</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1664,6 +1724,21 @@
       </c>
       <c r="B7">
         <v>5.49</v>
+      </c>
+      <c r="C7">
+        <v>3.3</v>
+      </c>
+      <c r="D7">
+        <v>3.96</v>
+      </c>
+      <c r="E7">
+        <v>4.76</v>
+      </c>
+      <c r="F7">
+        <v>5.58</v>
+      </c>
+      <c r="G7">
+        <v>6.24</v>
       </c>
     </row>
   </sheetData>
@@ -1679,7 +1754,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1728,6 +1803,21 @@
       <c r="B3">
         <v>43.66</v>
       </c>
+      <c r="C3">
+        <v>41.1</v>
+      </c>
+      <c r="D3">
+        <v>41.68</v>
+      </c>
+      <c r="E3">
+        <v>42.42</v>
+      </c>
+      <c r="F3">
+        <v>43.13</v>
+      </c>
+      <c r="G3">
+        <v>43.7</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1736,6 +1826,21 @@
       <c r="B4">
         <v>37.99</v>
       </c>
+      <c r="C4">
+        <v>37.03</v>
+      </c>
+      <c r="D4">
+        <v>37.61</v>
+      </c>
+      <c r="E4">
+        <v>38.32</v>
+      </c>
+      <c r="F4">
+        <v>39.04</v>
+      </c>
+      <c r="G4">
+        <v>39.700000000000003</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1744,6 +1849,21 @@
       <c r="B5">
         <v>11.76</v>
       </c>
+      <c r="C5">
+        <v>11.63</v>
+      </c>
+      <c r="D5">
+        <v>12.26</v>
+      </c>
+      <c r="E5">
+        <v>12.99</v>
+      </c>
+      <c r="F5">
+        <v>13.72</v>
+      </c>
+      <c r="G5">
+        <v>14.3</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1752,6 +1872,21 @@
       <c r="B6">
         <f>100-SUM(B3:B5)</f>
         <v>6.5899999999999892</v>
+      </c>
+      <c r="C6">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="D6">
+        <v>5.27</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>6.7</v>
+      </c>
+      <c r="G6">
+        <v>7.29</v>
       </c>
     </row>
   </sheetData>
@@ -1767,7 +1902,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,6 +1951,21 @@
       <c r="B3">
         <v>42.29</v>
       </c>
+      <c r="C3">
+        <v>40.11</v>
+      </c>
+      <c r="D3">
+        <v>40.69</v>
+      </c>
+      <c r="E3">
+        <v>41.44</v>
+      </c>
+      <c r="F3">
+        <v>42.2</v>
+      </c>
+      <c r="G3">
+        <v>42.79</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1824,6 +1974,21 @@
       <c r="B4">
         <v>43.38</v>
       </c>
+      <c r="C4">
+        <v>44.06</v>
+      </c>
+      <c r="D4">
+        <v>44.69</v>
+      </c>
+      <c r="E4">
+        <v>45.43</v>
+      </c>
+      <c r="F4">
+        <v>46.18</v>
+      </c>
+      <c r="G4">
+        <v>46.77</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1832,6 +1997,21 @@
       <c r="B5">
         <v>7.79</v>
       </c>
+      <c r="C5">
+        <v>6.45</v>
+      </c>
+      <c r="D5">
+        <v>7.14</v>
+      </c>
+      <c r="E5">
+        <v>7.99</v>
+      </c>
+      <c r="F5">
+        <v>8.83</v>
+      </c>
+      <c r="G5">
+        <v>9.5299999999999994</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1840,6 +2020,21 @@
       <c r="B6">
         <f>100-SUM(B3:B5)</f>
         <v>6.539999999999992</v>
+      </c>
+      <c r="C6">
+        <v>3.69</v>
+      </c>
+      <c r="D6">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="E6">
+        <v>5.26</v>
+      </c>
+      <c r="F6">
+        <v>6.15</v>
+      </c>
+      <c r="G6">
+        <v>6.9</v>
       </c>
     </row>
   </sheetData>
@@ -1854,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36A1C8C6-96C7-4DFE-8C83-4BC19ADE635C}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1904,6 +2099,21 @@
       <c r="B3">
         <v>41.58</v>
       </c>
+      <c r="C3">
+        <v>38.33</v>
+      </c>
+      <c r="D3">
+        <v>39.26</v>
+      </c>
+      <c r="E3">
+        <v>40.39</v>
+      </c>
+      <c r="F3">
+        <v>41.49</v>
+      </c>
+      <c r="G3">
+        <v>42.39</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1912,6 +2122,21 @@
       <c r="B4">
         <v>33.31</v>
       </c>
+      <c r="C4">
+        <v>32.4</v>
+      </c>
+      <c r="D4">
+        <v>33.28</v>
+      </c>
+      <c r="E4">
+        <v>34.43</v>
+      </c>
+      <c r="F4">
+        <v>35.590000000000003</v>
+      </c>
+      <c r="G4">
+        <v>36.49</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1920,6 +2145,21 @@
       <c r="B5">
         <v>9.57</v>
       </c>
+      <c r="C5">
+        <v>8.65</v>
+      </c>
+      <c r="D5">
+        <v>9.51</v>
+      </c>
+      <c r="E5">
+        <v>10.63</v>
+      </c>
+      <c r="F5">
+        <v>11.75</v>
+      </c>
+      <c r="G5">
+        <v>12.7</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1929,6 +2169,21 @@
         <f>100-SUM(B3:B5)</f>
         <v>15.539999999999992</v>
       </c>
+      <c r="C6">
+        <v>13.35</v>
+      </c>
+      <c r="D6">
+        <v>14.28</v>
+      </c>
+      <c r="E6">
+        <v>15.37</v>
+      </c>
+      <c r="F6">
+        <v>16.489999999999998</v>
+      </c>
+      <c r="G6">
+        <v>17.41</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1937,6 +2192,21 @@
       <c r="B7">
         <v>3.46</v>
       </c>
+      <c r="C7">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="D7">
+        <v>2.12</v>
+      </c>
+      <c r="E7">
+        <v>4.03</v>
+      </c>
+      <c r="F7">
+        <v>5.64</v>
+      </c>
+      <c r="G7">
+        <v>7.05</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1944,6 +2214,21 @@
       </c>
       <c r="B8">
         <v>1.1000000000000001</v>
+      </c>
+      <c r="C8">
+        <v>2.89</v>
+      </c>
+      <c r="D8">
+        <v>3.91</v>
+      </c>
+      <c r="E8">
+        <v>5.22</v>
+      </c>
+      <c r="F8">
+        <v>6.5</v>
+      </c>
+      <c r="G8">
+        <v>7.55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TPP series now includes random variations in the preference flows
</commit_message>
<xml_diff>
--- a/python/Model Election Comparisons.xlsx
+++ b/python/Model Election Comparisons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468F11E1-BA0E-490E-B125-2DEA534FAFF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6A979D-7AFD-483B-9F65-ED2939B515F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="12330" windowWidth="33540" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4860" yWindow="12015" windowWidth="33540" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sigmas" sheetId="30" r:id="rId1"/>
@@ -611,7 +611,7 @@
   <dimension ref="A2:AP61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AI10" sqref="AI10"/>
+      <selection activeCell="AF10" sqref="AF10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="AD5">
         <f>SUMPRODUCT(B5:AA5,B$19:AA$19)/SUM(B$19:AA$19)</f>
-        <v>0.93620631171554514</v>
+        <v>1.0114703530002402</v>
       </c>
       <c r="AE5">
         <f>SUMPRODUCT($B5:$AA5,$B$20:$AA$20)/SUM($B$20:$AA$20)</f>
@@ -1042,7 +1042,7 @@
       </c>
       <c r="AK5">
         <f>SQRT(SUMPRODUCT($B28:$AA28,$B$19:$AA$19)/(SUM($B$19:$AA$19)))</f>
-        <v>1.4500762773090998</v>
+        <v>1.5002272814478916</v>
       </c>
       <c r="AL5">
         <f>SQRT(SUMPRODUCT($B34:$AA34,$B$21:$AA$21)/(SUM($B$21:$AA$21)))</f>
@@ -1183,7 +1183,7 @@
       </c>
       <c r="AD6">
         <f t="shared" ref="AD6:AD8" si="2">SUMPRODUCT(B6:AA6,B$19:AA$19)/SUM(B$19:AA$19)</f>
-        <v>-0.15135129814079604</v>
+        <v>-0.30235198288909515</v>
       </c>
       <c r="AE6">
         <f t="shared" ref="AE6:AF8" si="3">SUMPRODUCT($B6:$AA6,$B$20:$AA$20)/SUM($B$20:$AA$20)</f>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="AK6">
         <f t="shared" ref="AK6:AK8" si="7">SQRT(SUMPRODUCT($B29:$AA29,$B$19:$AA$19)/(SUM($B$19:$AA$19)))</f>
-        <v>1.7128982814619305</v>
+        <v>1.7252852808042358</v>
       </c>
       <c r="AL6">
         <f t="shared" ref="AL6:AL8" si="8">SQRT(SUMPRODUCT($B35:$AA35,$B$21:$AA$21)/(SUM($B$21:$AA$21)))</f>
@@ -1352,7 +1352,7 @@
       </c>
       <c r="AD7">
         <f t="shared" si="2"/>
-        <v>-0.62152734391023268</v>
+        <v>-0.52644675836675037</v>
       </c>
       <c r="AE7">
         <f t="shared" si="3"/>
@@ -1380,7 +1380,7 @@
       </c>
       <c r="AK7">
         <f t="shared" si="7"/>
-        <v>1.2748624169190486</v>
+        <v>1.2993683484908121</v>
       </c>
       <c r="AL7">
         <f t="shared" si="8"/>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="AD8">
         <f t="shared" si="2"/>
-        <v>-0.46326359986532212</v>
+        <v>-0.5424072895984321</v>
       </c>
       <c r="AE8">
         <f t="shared" si="3"/>
@@ -1549,7 +1549,7 @@
       </c>
       <c r="AK8">
         <f t="shared" si="7"/>
-        <v>1.7518595728957513</v>
+        <v>1.8185192326700466</v>
       </c>
       <c r="AL8">
         <f t="shared" si="8"/>
@@ -1786,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -2527,107 +2527,107 @@
       </c>
       <c r="B28">
         <f>(B5-$AD5)^2</f>
-        <v>5.7888091670986945</v>
+        <v>5.4323041157300107</v>
       </c>
       <c r="C28">
         <f t="shared" ref="C28:AA28" si="21">(C5-$AD5)^2</f>
-        <v>0.56646759105043087</v>
+        <v>0.68542578517102115</v>
       </c>
       <c r="D28">
         <f t="shared" si="21"/>
-        <v>1.7432354950932451E-2</v>
+        <v>3.2225606894892892E-3</v>
       </c>
       <c r="E28">
         <f t="shared" si="21"/>
-        <v>0.14635402906551803</v>
+        <v>9.4432312734358675E-2</v>
       </c>
       <c r="F28">
         <f t="shared" si="21"/>
-        <v>0.10799840204194824</v>
+        <v>0.16313128780160641</v>
       </c>
       <c r="G28">
         <f t="shared" si="21"/>
-        <v>5.3504204014193139E-2</v>
+        <v>2.4350265616261389E-2</v>
       </c>
       <c r="H28">
         <f t="shared" si="21"/>
-        <v>4.0948090423501615E-2</v>
+        <v>7.7073078965570335E-2</v>
       </c>
       <c r="I28">
         <f t="shared" si="21"/>
-        <v>1.4549078049015303</v>
+        <v>1.6421387904009044</v>
       </c>
       <c r="J28">
         <f t="shared" si="21"/>
-        <v>0.99113466723021337</v>
+        <v>1.1466586995189521</v>
       </c>
       <c r="K28">
         <f t="shared" si="21"/>
-        <v>5.4602601855146045</v>
+        <v>5.1141828858920766</v>
       </c>
       <c r="L28">
         <f t="shared" si="21"/>
-        <v>13.970369650719979</v>
+        <v>14.538662503746679</v>
       </c>
       <c r="M28">
         <f t="shared" si="21"/>
-        <v>0.53225112409300046</v>
+        <v>0.42809722013673634</v>
       </c>
       <c r="N28">
         <f t="shared" si="21"/>
-        <v>0.31568446396927702</v>
+        <v>0.23677372552390075</v>
       </c>
       <c r="O28">
         <f t="shared" si="21"/>
-        <v>0.28041440180951344</v>
+        <v>0.36578997300764643</v>
       </c>
       <c r="P28">
         <f t="shared" si="21"/>
-        <v>0.20611542402522978</v>
+        <v>0.28011975393717303</v>
       </c>
       <c r="Q28">
         <f t="shared" si="21"/>
-        <v>0.45187190043994385</v>
+        <v>0.55872368756637214</v>
       </c>
       <c r="R28">
         <f t="shared" si="21"/>
-        <v>0.32763331901477277</v>
+        <v>0.41945915948800916</v>
       </c>
       <c r="S28">
         <f t="shared" si="21"/>
-        <v>3.6489149573622512</v>
+        <v>3.9421203827914892</v>
       </c>
       <c r="T28">
         <f t="shared" si="21"/>
-        <v>13.113391276850546</v>
+        <v>13.664154518787386</v>
       </c>
       <c r="U28">
         <f t="shared" si="21"/>
-        <v>1.6300561387175323</v>
+        <v>1.8279055147658239</v>
       </c>
       <c r="V28">
         <f t="shared" si="21"/>
-        <v>0.51496800328395331</v>
+        <v>0.6286535446396686</v>
       </c>
       <c r="W28">
         <f t="shared" si="21"/>
-        <v>0.48286541264990435</v>
+        <v>0.38393035488859423</v>
       </c>
       <c r="X28">
         <f t="shared" si="21"/>
-        <v>21.172123321313027</v>
+        <v>20.485160487078375</v>
       </c>
       <c r="Y28">
         <f t="shared" si="21"/>
-        <v>6.2649362182175747E-3</v>
+        <v>1.5111169607724271E-5</v>
       </c>
       <c r="Z28">
         <f t="shared" si="21"/>
-        <v>1.0710371316931468</v>
+        <v>1.2324847108909862</v>
       </c>
       <c r="AA28">
         <f t="shared" si="21"/>
-        <v>0.12625803752617573</v>
+        <v>0.1854095665384311</v>
       </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
@@ -2636,107 +2636,107 @@
       </c>
       <c r="B29">
         <f t="shared" ref="B29:AA29" si="22">(B6-$AD6)^2</f>
-        <v>5.3214510819729339</v>
+        <v>4.6475873576372448</v>
       </c>
       <c r="C29">
         <f t="shared" si="22"/>
-        <v>2.2801206794455231</v>
+        <v>2.7589460221290825</v>
       </c>
       <c r="D29">
         <f t="shared" si="22"/>
-        <v>5.2871039681668661E-2</v>
+        <v>0.14511354569264412</v>
       </c>
       <c r="E29">
         <f t="shared" si="22"/>
-        <v>1.2962801630342784E-2</v>
+        <v>7.0148162950331827E-2</v>
       </c>
       <c r="F29">
         <f t="shared" si="22"/>
-        <v>1.8435427214798712</v>
+        <v>1.4562951564099287</v>
       </c>
       <c r="G29">
         <f t="shared" si="22"/>
-        <v>1.0902595717301768</v>
+        <v>0.79772455190514635</v>
       </c>
       <c r="H29">
         <f t="shared" si="22"/>
-        <v>5.2251887139889277</v>
+        <v>4.5576549052794171</v>
       </c>
       <c r="I29">
         <f t="shared" si="22"/>
-        <v>2.0183055174825317</v>
+        <v>2.4701512510035681</v>
       </c>
       <c r="J29">
         <f t="shared" si="22"/>
-        <v>11.933610268433149</v>
+        <v>12.999676955409862</v>
       </c>
       <c r="K29">
         <f t="shared" si="22"/>
-        <v>23.162098174035791</v>
+        <v>21.731456860109642</v>
       </c>
       <c r="L29">
         <f t="shared" si="22"/>
-        <v>10.104217377057887</v>
+        <v>11.086994312525572</v>
       </c>
       <c r="M29">
         <f t="shared" si="22"/>
-        <v>0.65129432784471775</v>
+        <v>0.91781912113209407</v>
       </c>
       <c r="N29">
         <f t="shared" si="22"/>
-        <v>0.68655478020106486</v>
+        <v>0.95959009753272262</v>
       </c>
       <c r="O29">
         <f t="shared" si="22"/>
-        <v>1.0841559857550811</v>
+        <v>1.4214095089897114</v>
       </c>
       <c r="P29">
         <f t="shared" si="22"/>
-        <v>0.41081312706511275</v>
+        <v>0.24004744553319704</v>
       </c>
       <c r="Q29">
         <f t="shared" si="22"/>
-        <v>0.31565085467654619</v>
+        <v>0.50812492803871701</v>
       </c>
       <c r="R29">
         <f t="shared" si="22"/>
-        <v>3.3342651031215942</v>
+        <v>2.8056127103310584</v>
       </c>
       <c r="S29">
         <f t="shared" si="22"/>
-        <v>0.38718826360963543</v>
+        <v>0.59790817268727847</v>
       </c>
       <c r="T29">
         <f t="shared" si="22"/>
-        <v>6.2898994796069303</v>
+        <v>7.0701102156544939</v>
       </c>
       <c r="U29">
         <f t="shared" si="22"/>
-        <v>6.9465531463599088</v>
+        <v>7.7653186608939153</v>
       </c>
       <c r="V29">
         <f t="shared" si="22"/>
-        <v>4.7929566378941822E-2</v>
+        <v>0.13684739603254856</v>
       </c>
       <c r="W29">
         <f t="shared" si="22"/>
-        <v>2.8989313096913878</v>
+        <v>2.4075374862679535</v>
       </c>
       <c r="X29">
         <f t="shared" si="22"/>
-        <v>8.2432835787630676</v>
+        <v>9.1331645132520727</v>
       </c>
       <c r="Y29">
         <f t="shared" si="22"/>
-        <v>1.5264138214633072</v>
+        <v>1.9223320458117708</v>
       </c>
       <c r="Z29">
         <f t="shared" si="22"/>
-        <v>1.4123525622767181</v>
+        <v>1.7940595664005015</v>
       </c>
       <c r="AA29">
         <f t="shared" si="22"/>
-        <v>1.3365454375957871E-2</v>
+        <v>7.1080755122745407E-2</v>
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
@@ -2745,107 +2745,107 @@
       </c>
       <c r="B30">
         <f t="shared" ref="B30:AA30" si="23">(B7-$AD7)^2</f>
-        <v>0.8001587433239129</v>
+        <v>0.63909686487231199</v>
       </c>
       <c r="C30">
         <f t="shared" si="23"/>
-        <v>0.90403177472914231</v>
+        <v>1.0938784474222625</v>
       </c>
       <c r="D30">
         <f t="shared" si="23"/>
-        <v>2.9596729000283406</v>
+        <v>3.2958607896407086</v>
       </c>
       <c r="E30">
         <f t="shared" si="23"/>
-        <v>0.64837050617424508</v>
+        <v>0.81053136981642782</v>
       </c>
       <c r="F30">
         <f t="shared" si="23"/>
-        <v>3.3112293710552985E-2</v>
+        <v>7.5493944695331138E-3</v>
       </c>
       <c r="G30">
         <f t="shared" si="23"/>
-        <v>0.27181557113371269</v>
+        <v>0.18171358445528957</v>
       </c>
       <c r="H30">
         <f t="shared" si="23"/>
-        <v>0.43478660339226449</v>
+        <v>0.31843778210540102</v>
       </c>
       <c r="I30">
         <f t="shared" si="23"/>
-        <v>0.13801490036917377</v>
+        <v>0.21770077149948019</v>
       </c>
       <c r="J30">
         <f t="shared" si="23"/>
-        <v>2.2586532701698308</v>
+        <v>2.5534833235151262</v>
       </c>
       <c r="K30">
         <f t="shared" si="23"/>
-        <v>0.26933586278754562</v>
+        <v>0.17968713797508165</v>
       </c>
       <c r="L30">
         <f t="shared" si="23"/>
-        <v>2.3291598714683351E-2</v>
+        <v>6.1353525874489667E-2</v>
       </c>
       <c r="M30">
         <f t="shared" si="23"/>
-        <v>3.8503988463753882</v>
+        <v>4.2325816517867789</v>
       </c>
       <c r="N30">
         <f t="shared" si="23"/>
-        <v>10.836750133450582</v>
+        <v>11.471786184583962</v>
       </c>
       <c r="O30">
         <f t="shared" si="23"/>
-        <v>0.37468613201078099</v>
+        <v>0.50012716605966667</v>
       </c>
       <c r="P30">
         <f t="shared" si="23"/>
-        <v>1.099346471474669</v>
+        <v>0.90900332534900352</v>
       </c>
       <c r="Q30">
         <f t="shared" si="23"/>
-        <v>3.582447017696341</v>
+        <v>3.2315625691226044</v>
       </c>
       <c r="R30">
         <f t="shared" si="23"/>
-        <v>0.47277329512374427</v>
+        <v>0.35106162152325321</v>
       </c>
       <c r="S30">
         <f t="shared" si="23"/>
-        <v>1.012192322247641</v>
+        <v>0.82991572788847501</v>
       </c>
       <c r="T30">
         <f t="shared" si="23"/>
-        <v>8.5116399544758838</v>
+        <v>7.965890475132408</v>
       </c>
       <c r="U30">
         <f t="shared" si="23"/>
-        <v>1.6350130597794088</v>
+        <v>1.4008987963946382</v>
       </c>
       <c r="V30">
         <f t="shared" si="23"/>
-        <v>0.22331722220162625</v>
+        <v>0.14249411808784698</v>
       </c>
       <c r="W30">
         <f t="shared" si="23"/>
-        <v>1.8733802387420064</v>
+        <v>1.6221441448056846</v>
       </c>
       <c r="X30">
         <f t="shared" si="23"/>
-        <v>0.37418675136064256</v>
+        <v>0.49955019026838005</v>
       </c>
       <c r="Y30">
         <f t="shared" si="23"/>
-        <v>2.1871312838195203</v>
+        <v>1.9149431409816855</v>
       </c>
       <c r="Z30">
         <f t="shared" si="23"/>
-        <v>0.18118932988650913</v>
+        <v>0.27117429821907041</v>
       </c>
       <c r="AA30">
         <f t="shared" si="23"/>
-        <v>9.7048825607199536</v>
+        <v>9.1215202381994764</v>
       </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
@@ -2854,107 +2854,107 @@
       </c>
       <c r="B31">
         <f t="shared" ref="B31:AA31" si="24">(B8-$AD8)^2</f>
-        <v>0.39108569778350294</v>
+        <v>0.29836148831644321</v>
       </c>
       <c r="C31">
         <f t="shared" si="24"/>
-        <v>0.62637236245707884</v>
+        <v>0.75791055857306533</v>
       </c>
       <c r="D31">
         <f t="shared" si="24"/>
-        <v>2.8051193936937935</v>
+        <v>2.5462756476686277</v>
       </c>
       <c r="E31">
         <f t="shared" si="24"/>
-        <v>1.5931891020877638</v>
+        <v>1.799245680611161</v>
       </c>
       <c r="F31">
         <f t="shared" si="24"/>
-        <v>2.8731452841645955</v>
+        <v>3.1477117322870427</v>
       </c>
       <c r="G31">
         <f t="shared" si="24"/>
-        <v>1.9519211162436278E-2</v>
+        <v>4.7897449847585503E-2</v>
       </c>
       <c r="H31">
         <f t="shared" si="24"/>
-        <v>2.2754792990654624</v>
+        <v>2.5205146578796271</v>
       </c>
       <c r="I31">
         <f t="shared" si="24"/>
-        <v>2.0186588056277349E-2</v>
+        <v>4.8939705492828271E-2</v>
       </c>
       <c r="J31">
         <f t="shared" si="24"/>
-        <v>0.73362390284041912</v>
+        <v>0.60431156114708273</v>
       </c>
       <c r="K31">
         <f t="shared" si="24"/>
-        <v>2.7470723729052002</v>
+        <v>3.0156862603991459</v>
       </c>
       <c r="L31">
         <f t="shared" si="24"/>
-        <v>0.91883082562973428</v>
+        <v>1.0768219673366126</v>
       </c>
       <c r="M31">
         <f t="shared" si="24"/>
-        <v>0.93962404001762023</v>
+        <v>1.0993223790022588</v>
       </c>
       <c r="N31">
         <f t="shared" si="24"/>
-        <v>3.4986230838936851</v>
+        <v>3.8009571239233533</v>
       </c>
       <c r="O31">
         <f t="shared" si="24"/>
-        <v>0.12025666172477961</v>
+        <v>0.18141134974450449</v>
       </c>
       <c r="P31">
         <f t="shared" si="24"/>
-        <v>3.1200350084880715E-3</v>
+        <v>1.8225260087484929E-2</v>
       </c>
       <c r="Q31">
         <f t="shared" si="24"/>
-        <v>2.0166632989069457</v>
+        <v>1.7981442692058374</v>
       </c>
       <c r="R31">
         <f t="shared" si="24"/>
-        <v>4.6861957736975581</v>
+        <v>5.0351140474280518</v>
       </c>
       <c r="S31">
         <f t="shared" si="24"/>
-        <v>0.59435181741716125</v>
+        <v>0.7226459556122391</v>
       </c>
       <c r="T31">
         <f t="shared" si="24"/>
-        <v>6.1237637203818291</v>
+        <v>5.7383257029500445</v>
       </c>
       <c r="U31">
         <f t="shared" si="24"/>
-        <v>2.9294341309273517</v>
+        <v>2.6647796693187145</v>
       </c>
       <c r="V31">
         <f t="shared" si="24"/>
-        <v>3.7818749335330248E-2</v>
+        <v>1.3300257726852676E-2</v>
       </c>
       <c r="W31">
         <f t="shared" si="24"/>
-        <v>0.25942006241122367</v>
+        <v>0.34630476528097115</v>
       </c>
       <c r="X31">
         <f t="shared" si="24"/>
-        <v>62.355914401576563</v>
+        <v>61.112249784584975</v>
       </c>
       <c r="Y31">
         <f t="shared" si="24"/>
-        <v>9.3538919056610279</v>
+        <v>8.8760474029098422</v>
       </c>
       <c r="Z31">
         <f t="shared" si="24"/>
-        <v>1.4104287621819986</v>
+        <v>1.604676910251293</v>
       </c>
       <c r="AA31">
         <f t="shared" si="24"/>
-        <v>0.77810274140999347</v>
+        <v>0.64474095842902934</v>
       </c>
     </row>
     <row r="33" spans="1:27" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -12288,7 +12288,7 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>